<commit_message>
Added Javascript Tutorial Link
</commit_message>
<xml_diff>
--- a/Project and Tutorials/Python Resource list.xlsx
+++ b/Project and Tutorials/Python Resource list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Python" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,6 +16,7 @@
     <sheet name="Microbit" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Drawing, Image, Video" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="AI" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Javascript" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="174">
   <si>
     <t xml:space="preserve">Topic</t>
   </si>
@@ -500,6 +501,9 @@
     <t xml:space="preserve">https://youtu.be/P4Z8_qe2Cu0</t>
   </si>
   <si>
+    <t xml:space="preserve">You need to have some basic knowledge on Numpy array before starting OpenCV</t>
+  </si>
+  <si>
     <t xml:space="preserve">AI Intro from Raspberry Pi Site</t>
   </si>
   <si>
@@ -509,16 +513,25 @@
     <t xml:space="preserve">https://projects.raspberrypi.org/en/projects/testing-your-computers-vision/0</t>
   </si>
   <si>
+    <t xml:space="preserve">Introduction to AI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cats vs. Dogs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://projects.raspberrypi.org/en/projects/cats-vs-dogs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Improve your computer vision AI</t>
+  </si>
+  <si>
     <t xml:space="preserve">Teach your computer to read</t>
   </si>
   <si>
     <t xml:space="preserve">https://projects.raspberrypi.org/en/projects/teach-a-computer-to-read</t>
   </si>
   <si>
-    <t xml:space="preserve">Cats vs. Dogs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://projects.raspberrypi.org/en/projects/cats-vs-dogs</t>
+    <t xml:space="preserve">Text recgonition</t>
   </si>
   <si>
     <t xml:space="preserve">Rock, paper, scissors by hand</t>
@@ -528,6 +541,15 @@
   </si>
   <si>
     <t xml:space="preserve">Google Trainable Machine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you are solid on Python Basic, you can choose to learn Javascript. We will use a online full beginner course to learn Javascript. It is recommended that you learn some HTML and CSS before you start. To learn basic of HTML and CSS, go to the Web Programming tab and follow the “bird watch project. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Javascript full course from FreeCodeCamp:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Javascript full course on YouTube</t>
   </si>
 </sst>
 </file>
@@ -693,7 +715,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -786,7 +808,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -873,11 +907,11 @@
   </sheetPr>
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.38"/>
@@ -1155,7 +1189,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.87"/>
@@ -1422,9 +1456,9 @@
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1575,7 +1609,7 @@
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.74"/>
@@ -1696,7 +1730,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.25"/>
@@ -1768,7 +1802,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.2"/>
@@ -1808,13 +1842,13 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="25.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.23"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.63"/>
@@ -1930,12 +1964,16 @@
         <v>154</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="s">
+    <row r="11" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="23"/>
+      <c r="B11" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="24" t="s">
         <v>156</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -1962,69 +2000,79 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="33.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="46.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
-        <v>157</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="A1" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
     </row>
     <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="24" t="s">
-        <v>158</v>
+      <c r="A2" s="27" t="s">
+        <v>159</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="24" t="s">
-        <v>160</v>
+      <c r="A3" s="27" t="s">
+        <v>162</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>161</v>
+        <v>163</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="24" t="s">
-        <v>162</v>
+      <c r="A4" s="27" t="s">
+        <v>165</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>163</v>
+        <v>166</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="24" t="s">
-        <v>164</v>
+      <c r="A5" s="27" t="s">
+        <v>168</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>166</v>
-      </c>
-    </row>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="https://projects.raspberrypi.org/en/projects/testing-your-computers-vision/0"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://projects.raspberrypi.org/en/projects/teach-a-computer-to-read"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://projects.raspberrypi.org/en/projects/cats-vs-dogs"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://projects.raspberrypi.org/en/projects/cats-vs-dogs"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://projects.raspberrypi.org/en/projects/teach-a-computer-to-read"/>
     <hyperlink ref="B5" r:id="rId4" display="https://projects.raspberrypi.org/en/projects/rock-paper-scissors-by-hand"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2035,4 +2083,87 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.4"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>173</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H4"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" display="Javascript full course on YouTube"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>